<commit_message>
Solicitud de ingreso a sala y decisión del admin
Se agrega un alert para avisar al administrador de una sala que hay un usuario queriendo entrar.
El admin responde y si se aceptó la entrada, se agrega la sala a la lista de salas del solicitante, si se rechaza, surge un alert  informando el rechazo.
Se agrega tambien la funcionalidad en el lobby de los botones de sala, si se clickea sobre uno, se envía la solicitud de acceso.
Actualización de códigos de solicitud del server y el cliente
</commit_message>
<xml_diff>
--- a/RequestCodes.xlsx
+++ b/RequestCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herac\Documents\GitHub\Proyecto2P_Chatrooms_Heraclito\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7AB0D5-D887-40C1-8C7B-B9BB6F0D32C7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604BADF7-B3C5-4CB4-9C6D-9D5D04A82378}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3432" yWindow="636" windowWidth="14280" windowHeight="8952" activeTab="1" xr2:uid="{C26B2FFB-345C-4A78-B6E7-17B1AB578C10}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
   <si>
     <t>Petición</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>Salida de sala</t>
+  </si>
+  <si>
+    <t>Selección | Solicitante</t>
+  </si>
+  <si>
+    <t>Boolean | string</t>
   </si>
 </sst>
 </file>
@@ -486,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204BCBBA-238B-4E33-B50B-36D8865E5482}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,6 +544,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -555,6 +562,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -572,6 +580,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>31</v>
       </c>
@@ -657,8 +666,26 @@
         <v>28</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>109</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -751,6 +778,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -773,6 +801,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -784,6 +813,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
       <c r="B10" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Eliminar usuarios, cambio de admin, notificaciones
Se agrega la funcionalidad de que el administrador pueda eliminar usuarios, un recuadro en la parte superior de la sala de chat aparece en rojo cuando llegan nuevos mensajes a otras salas, y si el admin abandona la sala, el servidor elige al azar a otro usuario para ser el nuevo administrador y se le notifica
</commit_message>
<xml_diff>
--- a/RequestCodes.xlsx
+++ b/RequestCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herac\Documents\GitHub\Proyecto2P_Chatrooms_Heraclito\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604BADF7-B3C5-4CB4-9C6D-9D5D04A82378}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3735BCC6-4380-4427-AA56-4FAFADC06D40}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3432" yWindow="636" windowWidth="14280" windowHeight="8952" activeTab="1" xr2:uid="{C26B2FFB-345C-4A78-B6E7-17B1AB578C10}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
   <si>
     <t>Petición</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>Boolean | string</t>
+  </si>
+  <si>
+    <t>Desconexión de usuario</t>
+  </si>
+  <si>
+    <t>Usuario eliminado</t>
   </si>
 </sst>
 </file>
@@ -492,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204BCBBA-238B-4E33-B50B-36D8865E5482}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,6 +604,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>22</v>
       </c>
@@ -650,6 +657,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>27</v>
       </c>
@@ -667,6 +675,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -681,6 +690,20 @@
       </c>
       <c r="F10" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11">
+        <v>110</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -691,10 +714,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A8D1D9-70CE-4EFF-BA17-6A8B00B5C024}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,6 +767,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>17</v>
       </c>
@@ -755,6 +779,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -790,6 +815,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -835,6 +861,18 @@
         <v>7</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Agregar usuarios fuera de sala
El admin puede decidir agregar usuarios que no estén en la sala, al hacer click sobre el boton add, aparece una lista de botones con los nombres de los usuarios que aún no son miembros,  al dar click sobre ellos, se solicita confirmacion para agregar y si la respuesta es afirmativa, se agrega el usuario a la sala y se agrega la sala a la lista de salas del usuario
</commit_message>
<xml_diff>
--- a/RequestCodes.xlsx
+++ b/RequestCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herac\Documents\GitHub\Proyecto2P_Chatrooms_Heraclito\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3735BCC6-4380-4427-AA56-4FAFADC06D40}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7783C4E-4513-4640-AFB1-1B50E2B1A04F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3432" yWindow="636" windowWidth="14280" windowHeight="8952" activeTab="1" xr2:uid="{C26B2FFB-345C-4A78-B6E7-17B1AB578C10}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="36">
   <si>
     <t>Petición</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Respuesta de union a sala</t>
   </si>
   <si>
-    <t>Remoción de una sala</t>
-  </si>
-  <si>
     <t xml:space="preserve">Usuario </t>
   </si>
   <si>
@@ -100,21 +97,9 @@
     <t>Individual (Requester)</t>
   </si>
   <si>
-    <t>Salida de admin</t>
-  </si>
-  <si>
-    <t>Nuevo admin (random)</t>
-  </si>
-  <si>
-    <t>Individual (Nvo admin)</t>
-  </si>
-  <si>
     <t>Eliminar sala</t>
   </si>
   <si>
-    <t>Sala eliminada</t>
-  </si>
-  <si>
     <t>Eliminar usuario de sala</t>
   </si>
   <si>
@@ -140,6 +125,21 @@
   </si>
   <si>
     <t>Usuario eliminado</t>
+  </si>
+  <si>
+    <t>Agregar usuario a sala</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Usuario agregado por admin</t>
+  </si>
+  <si>
+    <t>Sala eliminada por admin</t>
+  </si>
+  <si>
+    <t>Notificación de usuario eliminado</t>
   </si>
 </sst>
 </file>
@@ -181,9 +181,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,7 +502,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,7 +526,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -543,7 +544,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -561,7 +562,7 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -576,19 +577,19 @@
         <v>103</v>
       </c>
       <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
         <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>104</v>
@@ -597,33 +598,33 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C6">
         <v>105</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>106</v>
@@ -632,7 +633,7 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
@@ -650,7 +651,7 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
@@ -659,7 +660,7 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>108</v>
@@ -668,10 +669,10 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -683,24 +684,24 @@
         <v>109</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C11">
         <v>110</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
@@ -714,10 +715,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A8D1D9-70CE-4EFF-BA17-6A8B00B5C024}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -779,9 +780,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+      <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C5">
         <v>13</v>
@@ -851,14 +852,15 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C11">
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -873,6 +875,18 @@
         <v>7</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Correciones a mensajes de alerta
Correcciones menores a mensajes de alertas
</commit_message>
<xml_diff>
--- a/RequestCodes.xlsx
+++ b/RequestCodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herac\Documents\GitHub\Proyecto2P_Chatrooms_Heraclito\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7783C4E-4513-4640-AFB1-1B50E2B1A04F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6AE98E0-1021-42EE-B14C-8AFC45DE8085}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3432" yWindow="636" windowWidth="14280" windowHeight="8952" activeTab="1" xr2:uid="{C26B2FFB-345C-4A78-B6E7-17B1AB578C10}"/>
+    <workbookView xWindow="3432" yWindow="636" windowWidth="14280" windowHeight="8952" xr2:uid="{C26B2FFB-345C-4A78-B6E7-17B1AB578C10}"/>
   </bookViews>
   <sheets>
     <sheet name="Server" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
   <si>
     <t>Petición</t>
   </si>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204BCBBA-238B-4E33-B50B-36D8865E5482}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -717,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A8D1D9-70CE-4EFF-BA17-6A8B00B5C024}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Admin puede borrar salas
Se agrega la función de que el administrador pueda borrar las salas
</commit_message>
<xml_diff>
--- a/RequestCodes.xlsx
+++ b/RequestCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herac\Documents\GitHub\Proyecto2P_Chatrooms_Heraclito\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6AE98E0-1021-42EE-B14C-8AFC45DE8085}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C3A2C0-CD91-4203-B767-A22E049497DF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3432" yWindow="636" windowWidth="14280" windowHeight="8952" xr2:uid="{C26B2FFB-345C-4A78-B6E7-17B1AB578C10}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="36">
   <si>
     <t>Petición</t>
   </si>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{204BCBBA-238B-4E33-B50B-36D8865E5482}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A687" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -699,6 +699,9 @@
       </c>
       <c r="C11">
         <v>110</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>

</xml_diff>